<commit_message>
Updated hours worked on tidsrapport
</commit_message>
<xml_diff>
--- a/doc/Tidrapport_Gr34.xlsx
+++ b/doc/Tidrapport_Gr34.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" state="visible" r:id="rId2"/>
@@ -356,7 +356,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -492,7 +492,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -521,11 +521,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="44937613"/>
-        <c:axId val="14896936"/>
+        <c:axId val="24584332"/>
+        <c:axId val="54115456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44937613"/>
+        <c:axId val="24584332"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,7 +557,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14896936"/>
+        <c:crossAx val="54115456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -565,7 +565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14896936"/>
+        <c:axId val="54115456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,7 +604,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44937613"/>
+        <c:crossAx val="24584332"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -667,9 +667,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>304200</xdr:colOff>
+      <xdr:colOff>303840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -677,8 +677,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3182400" y="457200"/>
-        <a:ext cx="4593600" cy="2628000"/>
+        <a:off x="3183120" y="457200"/>
+        <a:ext cx="4597560" cy="2627640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -698,11 +698,11 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -728,7 +728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
@@ -736,7 +736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
@@ -744,7 +744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
@@ -752,7 +752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
@@ -810,7 +810,7 @@
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -832,7 +832,7 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">v13!B8</f>
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,7 +904,7 @@
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">SUM(B2:B9)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -926,11 +926,11 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -967,24 +967,36 @@
         <f aca="false">Plan!A3</f>
         <v>Anton Wegeström</v>
       </c>
+      <c r="B3" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Plan!A4</f>
         <v>Rasmus Wallin</v>
       </c>
+      <c r="B4" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="str">
         <f aca="false">Plan!A5</f>
         <v>Jakob Österberg</v>
       </c>
+      <c r="B5" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="str">
         <f aca="false">Plan!A6</f>
         <v>Anton Östman</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -992,7 +1004,7 @@
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">SUM(B3:B6)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,7 +1059,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1134,7 +1146,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1221,7 +1233,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1304,7 +1316,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1390,7 +1402,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1473,7 +1485,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1556,7 +1568,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>

</xml_diff>

<commit_message>
Computer can now loop
</commit_message>
<xml_diff>
--- a/doc/Tidrapport_Gr34.xlsx
+++ b/doc/Tidrapport_Gr34.xlsx
@@ -492,7 +492,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>47</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -521,11 +521,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="47413222"/>
-        <c:axId val="76543018"/>
+        <c:axId val="96356312"/>
+        <c:axId val="38458742"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47413222"/>
+        <c:axId val="96356312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,7 +557,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76543018"/>
+        <c:crossAx val="38458742"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -565,7 +565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76543018"/>
+        <c:axId val="38458742"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,7 +604,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47413222"/>
+        <c:crossAx val="96356312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -667,9 +667,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>303480</xdr:colOff>
+      <xdr:colOff>303120</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>150840</xdr:rowOff>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -677,8 +677,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3184200" y="457200"/>
-        <a:ext cx="4606560" cy="2627280"/>
+        <a:off x="3184920" y="457200"/>
+        <a:ext cx="4610520" cy="2626920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -702,7 +702,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -810,7 +810,7 @@
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -832,7 +832,7 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">v13!B8</f>
-        <v>47</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,7 +904,7 @@
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">SUM(B2:B9)</f>
-        <v>47</v>
+        <v>62.5</v>
       </c>
     </row>
   </sheetData>
@@ -930,7 +930,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -968,7 +968,7 @@
         <v>Anton Wegeström</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>12</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -977,7 +977,7 @@
         <v>Rasmus Wallin</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>12</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,7 +986,7 @@
         <v>Jakob Österberg</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>11.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,7 +995,7 @@
         <v>Anton Östman</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">SUM(B3:B6)</f>
-        <v>47</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1059,7 +1059,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1146,7 +1146,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1233,7 +1233,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1316,7 +1316,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1402,7 +1402,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1485,7 +1485,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1568,7 +1568,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>

</xml_diff>

<commit_message>
Added Anton W's worked hours
</commit_message>
<xml_diff>
--- a/doc/Tidrapport_Gr34.xlsx
+++ b/doc/Tidrapport_Gr34.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" state="visible" r:id="rId2"/>
@@ -288,12 +288,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -370,18 +370,28 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
               <a:t>Arbetad tid</a:t>
@@ -390,12 +400,6 @@
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -427,27 +431,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -492,7 +481,7 @@
                   <c:v>65.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -518,11 +507,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="52729871"/>
-        <c:axId val="37517071"/>
+        <c:axId val="32217905"/>
+        <c:axId val="15251866"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52729871"/>
+        <c:axId val="32217905"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,27 +531,30 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37517071"/>
+        <c:crossAx val="15251866"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37517071"/>
+        <c:axId val="15251866"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -589,21 +581,24 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52729871"/>
+        <c:crossAx val="32217905"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -621,20 +616,6 @@
           <a:noFill/>
         </a:ln>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="595959"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -664,9 +645,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>302760</xdr:colOff>
+      <xdr:colOff>302400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>150120</xdr:rowOff>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -674,8 +655,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3184200" y="457200"/>
-        <a:ext cx="4605840" cy="2626560"/>
+        <a:off x="3184920" y="457200"/>
+        <a:ext cx="4609800" cy="2626200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -689,7 +670,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -699,10 +680,11 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -797,7 +779,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -807,10 +789,11 @@
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,7 +821,7 @@
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">v14!B8</f>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -901,7 +884,7 @@
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">SUM(B2:B9)</f>
-        <v>65.5</v>
+        <v>79.5</v>
       </c>
     </row>
   </sheetData>
@@ -917,20 +900,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,20 +1042,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1107,6 +1092,9 @@
         <f aca="false" t="array" ref="A3:A6">Plan!A3:A6</f>
         <v>Anton Wegeström</v>
       </c>
+      <c r="B3" s="0" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
@@ -1130,7 +1118,7 @@
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">SUM(B3:B6)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1145,7 +1133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1155,10 +1143,11 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1232,7 +1221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1242,10 +1231,11 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1315,7 +1305,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1325,10 +1315,11 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,7 +1392,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1411,10 +1402,11 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,7 +1476,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1494,10 +1486,11 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,7 +1560,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1577,10 +1570,11 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>